<commit_message>
delete test routes for ws and hr
</commit_message>
<xml_diff>
--- a/results_for_eccv/result.xlsx
+++ b/results_for_eccv/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoumengjie/Desktop/route-finder/results_for_eccv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF4BD3B-B39F-8C4B-9509-AAEFF0EE88FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA7FEE8-C4FF-3D4A-88DF-6DAE8DAC8C74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="460" windowWidth="25020" windowHeight="14000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3760" yWindow="460" windowWidth="25020" windowHeight="14000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSD_T_length " sheetId="1" r:id="rId1"/>
@@ -859,7 +859,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$7</c:f>
+              <c:f>'BSD_T_length '!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -936,7 +936,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$7:$I$7</c:f>
+              <c:f>'BSD_T_length '!$B$8:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -979,7 +979,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$8</c:f>
+              <c:f>'BSD_T_length '!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1056,7 +1056,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$8:$I$8</c:f>
+              <c:f>'BSD_T_length '!$B$9:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1099,7 +1099,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$9</c:f>
+              <c:f>'BSD_T_length '!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1176,7 +1176,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$9:$I$9</c:f>
+              <c:f>'BSD_T_length '!$B$10:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1219,7 +1219,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$10</c:f>
+              <c:f>'BSD_T_length '!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1296,7 +1296,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$10:$I$10</c:f>
+              <c:f>'BSD_T_length '!$B$11:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1547,7 +1547,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$19</c:f>
+              <c:f>'BSD_T_length '!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1591,7 +1591,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$18:$I$18</c:f>
+              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1624,7 +1624,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
+              <c:f>'BSD_T_length '!$B$20:$I$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1667,7 +1667,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$20</c:f>
+              <c:f>'BSD_T_length '!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1711,7 +1711,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$18:$I$18</c:f>
+              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1744,7 +1744,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$20:$I$20</c:f>
+              <c:f>'BSD_T_length '!$B$21:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1787,7 +1787,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$21</c:f>
+              <c:f>'BSD_T_length '!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1831,7 +1831,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$18:$I$18</c:f>
+              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1864,7 +1864,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$21:$I$21</c:f>
+              <c:f>'BSD_T_length '!$B$22:$I$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1907,7 +1907,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$22</c:f>
+              <c:f>'BSD_T_length '!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1951,7 +1951,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$18:$I$18</c:f>
+              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1984,7 +1984,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$22:$I$22</c:f>
+              <c:f>'BSD_T_length '!$B$23:$I$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2027,7 +2027,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$23</c:f>
+              <c:f>'BSD_T_length '!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2071,7 +2071,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$18:$I$18</c:f>
+              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2104,7 +2104,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$23:$I$23</c:f>
+              <c:f>'BSD_T_length '!$B$24:$I$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2147,7 +2147,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$24</c:f>
+              <c:f>'BSD_T_length '!$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2191,7 +2191,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$18:$I$18</c:f>
+              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2224,7 +2224,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$24:$I$24</c:f>
+              <c:f>'BSD_T_length '!$B$25:$I$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2267,7 +2267,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$25</c:f>
+              <c:f>'BSD_T_length '!$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2311,7 +2311,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$18:$I$18</c:f>
+              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2344,7 +2344,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$25:$I$25</c:f>
+              <c:f>'BSD_T_length '!$B$26:$I$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2387,7 +2387,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$26</c:f>
+              <c:f>'BSD_T_length '!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2431,7 +2431,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$18:$I$18</c:f>
+              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2464,7 +2464,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$26:$I$26</c:f>
+              <c:f>'BSD_T_length '!$B$27:$I$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2715,7 +2715,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$35</c:f>
+              <c:f>'BSD_T_length '!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2759,7 +2759,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$34:$I$34</c:f>
+              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2792,7 +2792,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
+              <c:f>'BSD_T_length '!$B$36:$I$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2835,7 +2835,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$36</c:f>
+              <c:f>'BSD_T_length '!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2879,7 +2879,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$34:$I$34</c:f>
+              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2912,7 +2912,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$36:$I$36</c:f>
+              <c:f>'BSD_T_length '!$B$37:$I$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2955,7 +2955,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$37</c:f>
+              <c:f>'BSD_T_length '!$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2999,7 +2999,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$34:$I$34</c:f>
+              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3032,7 +3032,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$37:$I$37</c:f>
+              <c:f>'BSD_T_length '!$B$38:$I$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3075,7 +3075,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$38</c:f>
+              <c:f>'BSD_T_length '!$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3119,7 +3119,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$34:$I$34</c:f>
+              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3152,7 +3152,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$38:$I$38</c:f>
+              <c:f>'BSD_T_length '!$B$39:$I$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3195,7 +3195,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$39</c:f>
+              <c:f>'BSD_T_length '!$A$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3239,7 +3239,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$34:$I$34</c:f>
+              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3272,7 +3272,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$39:$I$39</c:f>
+              <c:f>'BSD_T_length '!$B$40:$I$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3315,7 +3315,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$40</c:f>
+              <c:f>'BSD_T_length '!$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3359,7 +3359,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$34:$I$34</c:f>
+              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3392,7 +3392,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$40:$I$40</c:f>
+              <c:f>'BSD_T_length '!$B$41:$I$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3435,7 +3435,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$41</c:f>
+              <c:f>'BSD_T_length '!$A$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3479,7 +3479,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$34:$I$34</c:f>
+              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3512,7 +3512,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$41:$I$41</c:f>
+              <c:f>'BSD_T_length '!$B$42:$I$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3555,7 +3555,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$42</c:f>
+              <c:f>'BSD_T_length '!$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3599,7 +3599,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$34:$I$34</c:f>
+              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3632,7 +3632,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$42:$I$42</c:f>
+              <c:f>'BSD_T_length '!$B$43:$I$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7375,13 +7375,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>6480</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>196920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>437040</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7411,13 +7411,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>6480</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>197280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>437040</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7856,10 +7856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:I12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8023,363 +8023,361 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>80</v>
-      </c>
+      <c r="A7" s="2"/>
       <c r="B7" s="3">
-        <v>8.2000000000000003E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="C7" s="3">
-        <v>0.38400000000000001</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="D7" s="3">
-        <v>0.70199999999999996</v>
+        <v>0.59</v>
       </c>
       <c r="E7" s="3">
-        <v>0.88600000000000001</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="F7" s="3">
-        <v>0.95399999999999996</v>
+        <v>0.86599999999999999</v>
       </c>
       <c r="G7" s="3">
-        <v>0.96599999999999997</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="H7" s="3">
-        <v>0.97399999999999998</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="I7" s="3">
-        <v>0.96599999999999997</v>
+        <v>0.96399999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B8" s="3">
-        <v>0.17799999999999999</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="C8" s="3">
-        <v>0.74199999999999999</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="D8" s="3">
-        <v>0.93600000000000005</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="E8" s="3">
-        <v>0.97199999999999998</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="F8" s="3">
-        <v>0.98599999999999999</v>
+        <v>0.95399999999999996</v>
       </c>
       <c r="G8" s="3">
-        <v>0.99199999999999999</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="H8" s="3">
-        <v>0.996</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="I8" s="3">
-        <v>0.98</v>
+        <v>0.96599999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
+        <v>90</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.996</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>100</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="3">
         <v>0.48599999999999999</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C10" s="3">
         <v>0.92600000000000005</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="3">
         <v>0.97599999999999998</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E10" s="3">
         <v>0.98799999999999999</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F10" s="3">
         <v>0.99399999999999999</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G10" s="3">
         <v>0.996</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H10" s="3">
         <v>0.998</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I10" s="3">
         <v>0.98399999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B11" s="4">
         <v>0.126</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C11" s="4">
         <v>0.30399999999999999</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D11" s="4">
         <v>0.46400000000000002</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E11" s="4">
         <v>0.56200000000000006</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F11" s="4">
         <v>0.65400000000000003</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G11" s="4">
         <v>0.71799999999999997</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H11" s="4">
         <v>0.75</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I11" s="4">
         <v>0.76400000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="3">
         <v>0.11</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="3">
         <v>0.26400000000000001</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D13" s="3">
         <v>0.40400000000000003</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E13" s="3">
         <v>0.504</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F13" s="3">
         <v>0.61199999999999999</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G13" s="3">
         <v>0.68799999999999994</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H13" s="3">
         <v>0.74199999999999999</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I13" s="3">
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="1">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
         <v>5</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C19" s="1">
         <v>10</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D19" s="1">
         <v>15</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E19" s="1">
         <v>20</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F19" s="1">
         <v>25</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G19" s="1">
         <v>30</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H19" s="1">
         <v>35</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I19" s="1">
         <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>50</v>
-      </c>
-      <c r="B19" s="3">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="D19" s="3">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="E19" s="3">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="F19" s="3">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.128</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0.23599999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B20" s="3">
-        <v>6.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="C20" s="3">
-        <v>3.2000000000000001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="D20" s="3">
-        <v>0.112</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="E20" s="3">
-        <v>0.19600000000000001</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="F20" s="3">
-        <v>0.316</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="G20" s="3">
-        <v>0.41199999999999998</v>
+        <v>0.128</v>
       </c>
       <c r="H20" s="3">
-        <v>0.54</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="I20" s="3">
-        <v>0.64800000000000002</v>
+        <v>0.23599999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B21" s="3">
-        <v>0.03</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="C21" s="3">
-        <v>0.11799999999999999</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D21" s="3">
-        <v>0.27600000000000002</v>
+        <v>0.112</v>
       </c>
       <c r="E21" s="3">
-        <v>0.46600000000000003</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="F21" s="3">
-        <v>0.63600000000000001</v>
+        <v>0.316</v>
       </c>
       <c r="G21" s="3">
-        <v>0.77</v>
+        <v>0.41199999999999998</v>
       </c>
       <c r="H21" s="3">
-        <v>0.83199999999999996</v>
+        <v>0.54</v>
       </c>
       <c r="I21" s="3">
-        <v>0.88800000000000001</v>
+        <v>0.64800000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B22" s="3">
-        <v>3.2000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="C22" s="3">
-        <v>0.17399999999999999</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="D22" s="3">
-        <v>0.38800000000000001</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="E22" s="3">
-        <v>0.61399999999999999</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="F22" s="3">
-        <v>0.80400000000000005</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="G22" s="3">
-        <v>0.91400000000000003</v>
+        <v>0.77</v>
       </c>
       <c r="H22" s="3">
-        <v>0.95199999999999996</v>
+        <v>0.83199999999999996</v>
       </c>
       <c r="I22" s="3">
-        <v>0.96399999999999997</v>
+        <v>0.88800000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B23" s="3">
-        <v>5.1999999999999998E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="C23" s="3">
-        <v>0.26</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="D23" s="3">
-        <v>0.59599999999999997</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="E23" s="3">
-        <v>0.80200000000000005</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="F23" s="3">
-        <v>0.91800000000000004</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="G23" s="3">
-        <v>0.96599999999999997</v>
+        <v>0.91400000000000003</v>
       </c>
       <c r="H23" s="3">
-        <v>0.97599999999999998</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="I23" s="3">
-        <v>0.98799999999999999</v>
+        <v>0.96399999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B24" s="3">
-        <v>0.17199999999999999</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C24" s="3">
-        <v>0.60599999999999998</v>
+        <v>0.26</v>
       </c>
       <c r="D24" s="3">
-        <v>0.83599999999999997</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="E24" s="3">
-        <v>0.92200000000000004</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="F24" s="3">
-        <v>0.98199999999999998</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="G24" s="3">
-        <v>0.98799999999999999</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="H24" s="3">
-        <v>0.99399999999999999</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="I24" s="3">
         <v>0.98799999999999999</v>
@@ -8387,520 +8385,549 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
+        <v>90</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <v>100</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B26" s="3">
         <v>0.378</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C26" s="3">
         <v>0.83399999999999996</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D26" s="3">
         <v>0.93600000000000005</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E26" s="3">
         <v>0.97599999999999998</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F26" s="3">
         <v>0.998</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G26" s="3">
         <v>0.998</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H26" s="3">
         <v>0.996</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I26" s="3">
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B27" s="4">
         <v>0.16600000000000001</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C27" s="4">
         <v>0.38800000000000001</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D27" s="4">
         <v>0.59599999999999997</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E27" s="4">
         <v>0.77400000000000002</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F27" s="4">
         <v>0.878</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G27" s="4">
         <v>0.91800000000000004</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H27" s="4">
         <v>0.95599999999999996</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I27" s="4">
         <v>0.97599999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B29" s="3">
         <v>0.152</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C29" s="3">
         <v>0.38200000000000001</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D29" s="3">
         <v>0.60399999999999998</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E29" s="3">
         <v>0.77800000000000002</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F29" s="3">
         <v>0.83399999999999996</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G29" s="3">
         <v>0.89800000000000002</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H29" s="3">
         <v>0.94799999999999995</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I29" s="3">
         <v>0.97199999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="1">
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="1">
         <v>5</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C35" s="1">
         <v>10</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D35" s="1">
         <v>15</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E35" s="1">
         <v>20</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F35" s="1">
         <v>25</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G35" s="1">
         <v>30</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H35" s="1">
         <v>35</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I35" s="1">
         <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
-        <v>50</v>
-      </c>
-      <c r="B35" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="C35" s="3">
-        <v>1.6E-2</v>
-      </c>
-      <c r="D35" s="3">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0.06</v>
-      </c>
-      <c r="F35" s="3">
-        <v>0.09</v>
-      </c>
-      <c r="G35" s="3">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="H35" s="3">
-        <v>0.18</v>
-      </c>
-      <c r="I35" s="3">
-        <v>0.218</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B36" s="3">
-        <v>2E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C36" s="3">
-        <v>1.7999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D36" s="3">
-        <v>6.8000000000000005E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="E36" s="3">
-        <v>0.14399999999999999</v>
+        <v>0.06</v>
       </c>
       <c r="F36" s="3">
-        <v>0.2</v>
+        <v>0.09</v>
       </c>
       <c r="G36" s="3">
-        <v>0.27600000000000002</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="H36" s="3">
-        <v>0.34</v>
+        <v>0.18</v>
       </c>
       <c r="I36" s="3">
-        <v>0.41799999999999998</v>
+        <v>0.218</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B37" s="3">
-        <v>2.4E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="C37" s="3">
-        <v>0.11</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="D37" s="3">
-        <v>0.21</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="E37" s="3">
-        <v>0.35199999999999998</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="F37" s="3">
-        <v>0.48399999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="G37" s="3">
-        <v>0.61</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="H37" s="3">
-        <v>0.67400000000000004</v>
+        <v>0.34</v>
       </c>
       <c r="I37" s="3">
-        <v>0.74199999999999999</v>
+        <v>0.41799999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B38" s="3">
-        <v>3.2000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="C38" s="3">
-        <v>0.14799999999999999</v>
+        <v>0.11</v>
       </c>
       <c r="D38" s="3">
-        <v>0.35799999999999998</v>
+        <v>0.21</v>
       </c>
       <c r="E38" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="F38" s="3">
-        <v>0.68600000000000005</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="G38" s="3">
-        <v>0.746</v>
+        <v>0.61</v>
       </c>
       <c r="H38" s="3">
-        <v>0.82</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="I38" s="3">
-        <v>0.84</v>
+        <v>0.74199999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B39" s="3">
-        <v>0.04</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="C39" s="3">
-        <v>0.224</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="D39" s="3">
-        <v>0.45600000000000002</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="E39" s="3">
-        <v>0.628</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F39" s="3">
-        <v>0.72</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="G39" s="3">
-        <v>0.77</v>
+        <v>0.746</v>
       </c>
       <c r="H39" s="3">
-        <v>0.82599999999999996</v>
+        <v>0.82</v>
       </c>
       <c r="I39" s="3">
-        <v>0.86</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B40" s="3">
-        <v>9.4E-2</v>
+        <v>0.04</v>
       </c>
       <c r="C40" s="3">
-        <v>0.47199999999999998</v>
+        <v>0.224</v>
       </c>
       <c r="D40" s="3">
-        <v>0.69</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="E40" s="3">
-        <v>0.81200000000000006</v>
+        <v>0.628</v>
       </c>
       <c r="F40" s="3">
-        <v>0.86399999999999999</v>
+        <v>0.72</v>
       </c>
       <c r="G40" s="3">
-        <v>0.89200000000000002</v>
+        <v>0.77</v>
       </c>
       <c r="H40" s="3">
-        <v>0.91400000000000003</v>
+        <v>0.82599999999999996</v>
       </c>
       <c r="I40" s="3">
-        <v>0.92600000000000005</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
+        <v>90</v>
+      </c>
+      <c r="B41" s="3">
+        <v>9.4E-2</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0.92600000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
         <v>100</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B42" s="3">
         <v>0.25600000000000001</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C42" s="3">
         <v>0.64800000000000002</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D42" s="3">
         <v>0.79400000000000004</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E42" s="3">
         <v>0.874</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F42" s="3">
         <v>0.89600000000000002</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G42" s="3">
         <v>0.91800000000000004</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H42" s="3">
         <v>0.93400000000000005</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I42" s="3">
         <v>0.94199999999999995</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B43" s="4">
         <v>0.04</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C43" s="4">
         <v>0.08</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D43" s="4">
         <v>0.16800000000000001</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E43" s="4">
         <v>0.26400000000000001</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F43" s="4">
         <v>0.318</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G43" s="4">
         <v>0.40400000000000003</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H43" s="4">
         <v>0.48199999999999998</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I43" s="4">
         <v>0.53200000000000003</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B45" s="3">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C45" s="3">
         <v>0.106</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D45" s="3">
         <v>0.216</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E45" s="3">
         <v>0.28799999999999998</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F45" s="3">
         <v>0.35199999999999998</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G45" s="3">
         <v>0.42399999999999999</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H45" s="3">
         <v>0.504</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I45" s="3">
         <v>0.55800000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="13" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="8"/>
+      <c r="B49" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B50" s="3">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C50" s="3">
         <v>0.152</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D50" s="3">
         <v>0.312</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E50" s="3">
         <v>0.5</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F50" s="3">
         <v>0.63200000000000001</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G50" s="3">
         <v>0.71199999999999997</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H50" s="3">
         <v>0.77200000000000002</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I50" s="3">
         <v>0.79400000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B51" s="6">
         <v>0.11</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C51" s="6">
         <v>0.29199999999999998</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="6">
         <v>0.45800000000000002</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E51" s="6">
         <v>0.57799999999999996</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F51" s="6">
         <v>0.67400000000000004</v>
       </c>
-      <c r="G50" s="6">
+      <c r="G51" s="6">
         <v>0.70599999999999996</v>
       </c>
-      <c r="H50" s="6">
+      <c r="H51" s="6">
         <v>0.72799999999999998</v>
       </c>
-      <c r="I50" s="6">
+      <c r="I51" s="6">
         <v>0.76800000000000002</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B53" s="3">
         <v>0.12</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C53" s="3">
         <v>0.28799999999999998</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D53" s="3">
         <v>0.45200000000000001</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E53" s="3">
         <v>0.54600000000000004</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F53" s="3">
         <v>0.63200000000000001</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G53" s="3">
         <v>0.67400000000000004</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H53" s="3">
         <v>0.71199999999999997</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I53" s="3">
         <v>0.76200000000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="B49:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9750,7 +9777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F0FACB-EA77-744D-9F1B-27813583D2CB}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
results.xlsx for new test routes
</commit_message>
<xml_diff>
--- a/results_for_eccv/result.xlsx
+++ b/results_for_eccv/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoumengjie/Desktop/route-finder/results_for_eccv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA7FEE8-C4FF-3D4A-88DF-6DAE8DAC8C74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734BE8E7-82D9-104E-B807-B7E826F984F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="460" windowWidth="25020" windowHeight="14000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="14000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSD_T_length " sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="32">
   <si>
     <t>wall street with turns</t>
   </si>
@@ -118,7 +118,16 @@
     <t>cmu</t>
   </si>
   <si>
-    <t>hudson river</t>
+    <t>old test routes</t>
+  </si>
+  <si>
+    <t>hudsonriver</t>
+  </si>
+  <si>
+    <t>new test routes</t>
+  </si>
+  <si>
+    <t>wall street with turns (new test routes)</t>
   </si>
 </sst>
 </file>
@@ -155,7 +164,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +201,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -205,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -235,13 +250,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,7 +877,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$8</c:f>
+              <c:f>'BSD_T_length '!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -936,7 +954,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$8:$I$8</c:f>
+              <c:f>'BSD_T_length '!$B$7:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -979,7 +997,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$9</c:f>
+              <c:f>'BSD_T_length '!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1056,7 +1074,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$9:$I$9</c:f>
+              <c:f>'BSD_T_length '!$B$8:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1099,7 +1117,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$10</c:f>
+              <c:f>'BSD_T_length '!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1176,7 +1194,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$10:$I$10</c:f>
+              <c:f>'BSD_T_length '!$B$9:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1219,7 +1237,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$11</c:f>
+              <c:f>'BSD_T_length '!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1296,7 +1314,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$11:$I$11</c:f>
+              <c:f>'BSD_T_length '!$B$10:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1547,7 +1565,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$20</c:f>
+              <c:f>'BSD_T_length '!$A$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1591,7 +1609,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
+              <c:f>'BSD_T_length '!$B$32:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1624,7 +1642,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$20:$I$20</c:f>
+              <c:f>'BSD_T_length '!$B$33:$I$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1667,7 +1685,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$21</c:f>
+              <c:f>'BSD_T_length '!$A$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1711,7 +1729,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
+              <c:f>'BSD_T_length '!$B$32:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1744,7 +1762,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$21:$I$21</c:f>
+              <c:f>'BSD_T_length '!$B$34:$I$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1787,7 +1805,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$22</c:f>
+              <c:f>'BSD_T_length '!$A$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1831,7 +1849,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
+              <c:f>'BSD_T_length '!$B$32:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1864,7 +1882,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$22:$I$22</c:f>
+              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1907,7 +1925,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$23</c:f>
+              <c:f>'BSD_T_length '!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1951,7 +1969,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
+              <c:f>'BSD_T_length '!$B$32:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1984,7 +2002,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$23:$I$23</c:f>
+              <c:f>'BSD_T_length '!$B$36:$I$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2027,7 +2045,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$24</c:f>
+              <c:f>'BSD_T_length '!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2071,7 +2089,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
+              <c:f>'BSD_T_length '!$B$32:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2104,7 +2122,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$24:$I$24</c:f>
+              <c:f>'BSD_T_length '!$B$37:$I$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2147,7 +2165,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$25</c:f>
+              <c:f>'BSD_T_length '!$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2191,7 +2209,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
+              <c:f>'BSD_T_length '!$B$32:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2224,7 +2242,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$25:$I$25</c:f>
+              <c:f>'BSD_T_length '!$B$38:$I$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2267,7 +2285,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$26</c:f>
+              <c:f>'BSD_T_length '!$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2311,7 +2329,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
+              <c:f>'BSD_T_length '!$B$32:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2344,7 +2362,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$26:$I$26</c:f>
+              <c:f>'BSD_T_length '!$B$39:$I$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2387,7 +2405,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$27</c:f>
+              <c:f>'BSD_T_length '!$A$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2431,7 +2449,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$19:$I$19</c:f>
+              <c:f>'BSD_T_length '!$B$32:$I$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2464,7 +2482,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$27:$I$27</c:f>
+              <c:f>'BSD_T_length '!$B$40:$I$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2715,7 +2733,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$36</c:f>
+              <c:f>'BSD_T_length '!$A$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2759,7 +2777,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
+              <c:f>'BSD_T_length '!$B$48:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2792,7 +2810,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$36:$I$36</c:f>
+              <c:f>'BSD_T_length '!$B$49:$I$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2835,7 +2853,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$37</c:f>
+              <c:f>'BSD_T_length '!$A$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2879,7 +2897,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
+              <c:f>'BSD_T_length '!$B$48:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2912,7 +2930,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$37:$I$37</c:f>
+              <c:f>'BSD_T_length '!$B$50:$I$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2955,7 +2973,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$38</c:f>
+              <c:f>'BSD_T_length '!$A$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2999,7 +3017,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
+              <c:f>'BSD_T_length '!$B$48:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3032,7 +3050,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$38:$I$38</c:f>
+              <c:f>'BSD_T_length '!$B$51:$I$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3075,7 +3093,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$39</c:f>
+              <c:f>'BSD_T_length '!$A$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3119,7 +3137,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
+              <c:f>'BSD_T_length '!$B$48:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3152,7 +3170,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$39:$I$39</c:f>
+              <c:f>'BSD_T_length '!$B$52:$I$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3195,7 +3213,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$40</c:f>
+              <c:f>'BSD_T_length '!$A$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3239,7 +3257,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
+              <c:f>'BSD_T_length '!$B$48:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3272,7 +3290,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$40:$I$40</c:f>
+              <c:f>'BSD_T_length '!$B$53:$I$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3315,7 +3333,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$41</c:f>
+              <c:f>'BSD_T_length '!$A$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3359,7 +3377,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
+              <c:f>'BSD_T_length '!$B$48:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3392,7 +3410,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$41:$I$41</c:f>
+              <c:f>'BSD_T_length '!$B$54:$I$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3435,7 +3453,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$42</c:f>
+              <c:f>'BSD_T_length '!$A$55</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3479,7 +3497,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
+              <c:f>'BSD_T_length '!$B$48:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3512,7 +3530,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$42:$I$42</c:f>
+              <c:f>'BSD_T_length '!$B$55:$I$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3555,7 +3573,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BSD_T_length '!$A$43</c:f>
+              <c:f>'BSD_T_length '!$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3599,7 +3617,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
+              <c:f>'BSD_T_length '!$B$48:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3632,7 +3650,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BSD_T_length '!$B$43:$I$43</c:f>
+              <c:f>'BSD_T_length '!$B$56:$I$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7375,13 +7393,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>6480</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>196920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>437040</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7411,13 +7429,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>6480</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>197280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>437040</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7856,10 +7874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:I7"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7868,17 +7886,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -8023,911 +8041,1116 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2">
+        <v>80</v>
+      </c>
       <c r="B7" s="3">
-        <v>6.8000000000000005E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="C7" s="3">
-        <v>0.30399999999999999</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="D7" s="3">
-        <v>0.59</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="E7" s="3">
-        <v>0.75800000000000001</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="F7" s="3">
-        <v>0.86599999999999999</v>
+        <v>0.95399999999999996</v>
       </c>
       <c r="G7" s="3">
-        <v>0.92800000000000005</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="H7" s="3">
-        <v>0.95199999999999996</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="I7" s="3">
-        <v>0.96399999999999997</v>
+        <v>0.96599999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B8" s="3">
-        <v>8.2000000000000003E-2</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="C8" s="3">
-        <v>0.38400000000000001</v>
+        <v>0.74199999999999999</v>
       </c>
       <c r="D8" s="3">
-        <v>0.70199999999999996</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="E8" s="3">
-        <v>0.88600000000000001</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="F8" s="3">
-        <v>0.95399999999999996</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="G8" s="3">
-        <v>0.96599999999999997</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="H8" s="3">
-        <v>0.97399999999999998</v>
+        <v>0.996</v>
       </c>
       <c r="I8" s="3">
-        <v>0.96599999999999997</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B9" s="3">
-        <v>0.17799999999999999</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="C9" s="3">
-        <v>0.74199999999999999</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="D9" s="3">
-        <v>0.93600000000000005</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="E9" s="3">
-        <v>0.97199999999999998</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="F9" s="3">
-        <v>0.98599999999999999</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="G9" s="3">
-        <v>0.99199999999999999</v>
+        <v>0.996</v>
       </c>
       <c r="H9" s="3">
-        <v>0.996</v>
+        <v>0.998</v>
       </c>
       <c r="I9" s="3">
-        <v>0.98</v>
+        <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>100</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.996</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0.998</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0.98399999999999999</v>
+      <c r="A10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.126</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.76400000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0.126</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.46400000000000002</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0.56200000000000006</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0.71799999999999997</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0.76400000000000001</v>
+      <c r="A11" s="5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B12" s="3">
         <v>0.11</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C12" s="3">
         <v>0.26400000000000001</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D12" s="3">
         <v>0.40400000000000003</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E12" s="3">
         <v>0.504</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F12" s="3">
         <v>0.61199999999999999</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G12" s="3">
         <v>0.68799999999999994</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H12" s="3">
         <v>0.74199999999999999</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I12" s="3">
         <v>0.76800000000000002</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1">
+        <v>20</v>
+      </c>
+      <c r="F17" s="1">
+        <v>25</v>
+      </c>
+      <c r="G17" s="1">
+        <v>30</v>
+      </c>
+      <c r="H17" s="1">
+        <v>35</v>
+      </c>
+      <c r="I17" s="1">
+        <v>40</v>
+      </c>
+    </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+      <c r="A18" s="2">
+        <v>50</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="1">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1">
-        <v>10</v>
-      </c>
-      <c r="D19" s="1">
-        <v>15</v>
-      </c>
-      <c r="E19" s="1">
-        <v>20</v>
-      </c>
-      <c r="F19" s="1">
-        <v>25</v>
-      </c>
-      <c r="G19" s="1">
-        <v>30</v>
-      </c>
-      <c r="H19" s="1">
-        <v>35</v>
-      </c>
-      <c r="I19" s="1">
-        <v>40</v>
-      </c>
+      <c r="A19" s="2">
+        <v>60</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>50</v>
-      </c>
-      <c r="B20" s="3">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="D20" s="3">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="E20" s="3">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="F20" s="3">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0.128</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0.23599999999999999</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>60</v>
-      </c>
-      <c r="B21" s="3">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="C21" s="3">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0.112</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0.19600000000000001</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0.316</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0.41199999999999998</v>
-      </c>
-      <c r="H21" s="3">
-        <v>0.54</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0.64800000000000002</v>
+        <v>75</v>
+      </c>
+      <c r="B21" s="4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.246</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.96199999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>70</v>
-      </c>
-      <c r="B22" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0.63600000000000001</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0.77</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0.83199999999999996</v>
-      </c>
-      <c r="I22" s="3">
-        <v>0.88800000000000001</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>75</v>
-      </c>
-      <c r="B23" s="3">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0.17399999999999999</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0.61399999999999999</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0.80400000000000005</v>
-      </c>
-      <c r="G23" s="3">
-        <v>0.91400000000000003</v>
-      </c>
-      <c r="H23" s="3">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="I23" s="3">
-        <v>0.96399999999999997</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>80</v>
-      </c>
-      <c r="B24" s="3">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0.80200000000000005</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.91800000000000004</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0.96599999999999997</v>
-      </c>
-      <c r="H24" s="3">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="I24" s="3">
-        <v>0.98799999999999999</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>90</v>
-      </c>
-      <c r="B25" s="3">
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0.60599999999999998</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0.83599999999999997</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="I25" s="3">
-        <v>0.98799999999999999</v>
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.126</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0.76400000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>100</v>
-      </c>
-      <c r="B26" s="3">
-        <v>0.378</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0.83399999999999996</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0.998</v>
-      </c>
-      <c r="G26" s="3">
-        <v>0.998</v>
-      </c>
-      <c r="H26" s="3">
-        <v>0.996</v>
-      </c>
-      <c r="I26" s="3">
-        <v>0.99199999999999999</v>
+      <c r="A26" s="5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0.76800000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="1">
         <v>5</v>
       </c>
-      <c r="B27" s="4">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="E27" s="4">
-        <v>0.77400000000000002</v>
-      </c>
-      <c r="F27" s="4">
-        <v>0.878</v>
-      </c>
-      <c r="G27" s="4">
-        <v>0.91800000000000004</v>
-      </c>
-      <c r="H27" s="4">
-        <v>0.95599999999999996</v>
-      </c>
-      <c r="I27" s="4">
-        <v>0.97599999999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="3">
-        <v>0.152</v>
-      </c>
-      <c r="C29" s="3">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="E29" s="3">
-        <v>0.77800000000000002</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0.83399999999999996</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0.89800000000000002</v>
-      </c>
-      <c r="H29" s="3">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="I29" s="3">
-        <v>0.97199999999999998</v>
+      <c r="C32" s="1">
+        <v>10</v>
+      </c>
+      <c r="D32" s="1">
+        <v>15</v>
+      </c>
+      <c r="E32" s="1">
+        <v>20</v>
+      </c>
+      <c r="F32" s="1">
+        <v>25</v>
+      </c>
+      <c r="G32" s="1">
+        <v>30</v>
+      </c>
+      <c r="H32" s="1">
+        <v>35</v>
+      </c>
+      <c r="I32" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>50</v>
+      </c>
+      <c r="B33" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D33" s="3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E33" s="3">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F33" s="3">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0.128</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0.23599999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
+      <c r="A34" s="2">
+        <v>60</v>
+      </c>
+      <c r="B34" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C34" s="3">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.112</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.316</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0.64800000000000002</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="1">
-        <v>5</v>
-      </c>
-      <c r="C35" s="1">
-        <v>10</v>
-      </c>
-      <c r="D35" s="1">
-        <v>15</v>
-      </c>
-      <c r="E35" s="1">
-        <v>20</v>
-      </c>
-      <c r="F35" s="1">
-        <v>25</v>
-      </c>
-      <c r="G35" s="1">
-        <v>30</v>
-      </c>
-      <c r="H35" s="1">
-        <v>35</v>
-      </c>
-      <c r="I35" s="1">
-        <v>40</v>
+      <c r="A35" s="2">
+        <v>70</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0.88800000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="B36" s="3">
-        <v>8.0000000000000002E-3</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="C36" s="3">
-        <v>1.6E-2</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="D36" s="3">
-        <v>3.5999999999999997E-2</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="E36" s="3">
-        <v>0.06</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="F36" s="3">
-        <v>0.09</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="G36" s="3">
-        <v>0.11600000000000001</v>
+        <v>0.91400000000000003</v>
       </c>
       <c r="H36" s="3">
-        <v>0.18</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="I36" s="3">
-        <v>0.218</v>
+        <v>0.96399999999999997</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B37" s="3">
-        <v>2E-3</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C37" s="3">
-        <v>1.7999999999999999E-2</v>
+        <v>0.26</v>
       </c>
       <c r="D37" s="3">
-        <v>6.8000000000000005E-2</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="E37" s="3">
-        <v>0.14399999999999999</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="F37" s="3">
-        <v>0.2</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="G37" s="3">
-        <v>0.27600000000000002</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="H37" s="3">
-        <v>0.34</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="I37" s="3">
-        <v>0.41799999999999998</v>
+        <v>0.98799999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="B38" s="3">
-        <v>2.4E-2</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="C38" s="3">
-        <v>0.11</v>
+        <v>0.60599999999999998</v>
       </c>
       <c r="D38" s="3">
-        <v>0.21</v>
+        <v>0.83599999999999997</v>
       </c>
       <c r="E38" s="3">
-        <v>0.35199999999999998</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="F38" s="3">
-        <v>0.48399999999999999</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="G38" s="3">
-        <v>0.61</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="H38" s="3">
-        <v>0.67400000000000004</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="I38" s="3">
-        <v>0.74199999999999999</v>
+        <v>0.98799999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
+        <v>100</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0.378</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.998</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0.998</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0.996</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0.878</v>
+      </c>
+      <c r="G40" s="4">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0.152</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="I42" s="3">
+        <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="1">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1">
+        <v>10</v>
+      </c>
+      <c r="D48" s="1">
+        <v>15</v>
+      </c>
+      <c r="E48" s="1">
+        <v>20</v>
+      </c>
+      <c r="F48" s="1">
+        <v>25</v>
+      </c>
+      <c r="G48" s="1">
+        <v>30</v>
+      </c>
+      <c r="H48" s="1">
+        <v>35</v>
+      </c>
+      <c r="I48" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>50</v>
+      </c>
+      <c r="B49" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C49" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D49" s="3">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="I49" s="3">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>60</v>
+      </c>
+      <c r="B50" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D50" s="3">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0.41799999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>70</v>
+      </c>
+      <c r="B51" s="3">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
         <v>75</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B52" s="3">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C52" s="3">
         <v>0.14799999999999999</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D52" s="3">
         <v>0.35799999999999998</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E52" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F52" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G52" s="3">
         <v>0.746</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H52" s="3">
         <v>0.82</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I52" s="3">
         <v>0.84</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
         <v>80</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B53" s="3">
         <v>0.04</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C53" s="3">
         <v>0.224</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D53" s="3">
         <v>0.45600000000000002</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E53" s="3">
         <v>0.628</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F53" s="3">
         <v>0.72</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G53" s="3">
         <v>0.77</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H53" s="3">
         <v>0.82599999999999996</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I53" s="3">
         <v>0.86</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
         <v>90</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B54" s="3">
         <v>9.4E-2</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C54" s="3">
         <v>0.47199999999999998</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D54" s="3">
         <v>0.69</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E54" s="3">
         <v>0.81200000000000006</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F54" s="3">
         <v>0.86399999999999999</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G54" s="3">
         <v>0.89200000000000002</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H54" s="3">
         <v>0.91400000000000003</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I54" s="3">
         <v>0.92600000000000005</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
         <v>100</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B55" s="3">
         <v>0.25600000000000001</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C55" s="3">
         <v>0.64800000000000002</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D55" s="3">
         <v>0.79400000000000004</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E55" s="3">
         <v>0.874</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F55" s="3">
         <v>0.89600000000000002</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G55" s="3">
         <v>0.91800000000000004</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H55" s="3">
         <v>0.93400000000000005</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I55" s="3">
         <v>0.94199999999999995</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B56" s="4">
         <v>0.04</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C56" s="4">
         <v>0.08</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D56" s="4">
         <v>0.16800000000000001</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E56" s="4">
         <v>0.26400000000000001</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F56" s="4">
         <v>0.318</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G56" s="4">
         <v>0.40400000000000003</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H56" s="4">
         <v>0.48199999999999998</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I56" s="4">
         <v>0.53200000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B58" s="3">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C58" s="3">
         <v>0.106</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D58" s="3">
         <v>0.216</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E58" s="3">
         <v>0.28799999999999998</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F58" s="3">
         <v>0.35199999999999998</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G58" s="3">
         <v>0.42399999999999999</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H58" s="3">
         <v>0.504</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I58" s="3">
         <v>0.55800000000000005</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="8"/>
-      <c r="B49" s="13" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="8"/>
+      <c r="B62" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B63" s="3">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C63" s="3">
         <v>0.152</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D63" s="3">
         <v>0.312</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E63" s="3">
         <v>0.5</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F63" s="3">
         <v>0.63200000000000001</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G63" s="3">
         <v>0.71199999999999997</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H63" s="3">
         <v>0.77200000000000002</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I63" s="3">
         <v>0.79400000000000004</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B64" s="6">
         <v>0.11</v>
       </c>
-      <c r="C51" s="6">
+      <c r="C64" s="6">
         <v>0.29199999999999998</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D64" s="6">
         <v>0.45800000000000002</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E64" s="6">
         <v>0.57799999999999996</v>
       </c>
-      <c r="F51" s="6">
+      <c r="F64" s="6">
         <v>0.67400000000000004</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G64" s="6">
         <v>0.70599999999999996</v>
       </c>
-      <c r="H51" s="6">
+      <c r="H64" s="6">
         <v>0.72799999999999998</v>
       </c>
-      <c r="I51" s="6">
+      <c r="I64" s="6">
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B66" s="3">
         <v>0.12</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C66" s="3">
         <v>0.28799999999999998</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D66" s="3">
         <v>0.45200000000000001</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E66" s="3">
         <v>0.54600000000000004</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F66" s="3">
         <v>0.63200000000000001</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G66" s="3">
         <v>0.67400000000000004</v>
       </c>
-      <c r="H53" s="3">
+      <c r="H66" s="3">
         <v>0.71199999999999997</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I66" s="3">
         <v>0.76200000000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="B49:I49"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A47:I47"/>
+    <mergeCell ref="B62:I62"/>
+    <mergeCell ref="A16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -8949,17 +9172,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -9220,17 +9443,17 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -9491,17 +9714,17 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B35" s="1">
@@ -9775,15 +9998,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F0FACB-EA77-744D-9F1B-27813583D2CB}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -9811,6 +10035,9 @@
       <c r="I1" s="10">
         <v>40</v>
       </c>
+      <c r="J1" s="13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -9840,7 +10067,7 @@
       <c r="I2" s="3">
         <v>0.30599999999999999</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -9870,7 +10097,7 @@
       <c r="I3" s="3">
         <v>0.246</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -9900,12 +10127,10 @@
       <c r="I4" s="3">
         <v>0.25800000000000001</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>28</v>
-      </c>
+      <c r="A5" s="14"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -9917,7 +10142,7 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -9929,21 +10154,137 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
+      <c r="A7" s="14"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="10">
+        <v>5</v>
+      </c>
+      <c r="C10" s="10">
+        <v>10</v>
+      </c>
+      <c r="D10" s="10">
+        <v>15</v>
+      </c>
+      <c r="E10" s="10">
+        <v>20</v>
+      </c>
+      <c r="F10" s="10">
+        <v>25</v>
+      </c>
+      <c r="G10" s="10">
+        <v>30</v>
+      </c>
+      <c r="H10" s="10">
+        <v>35</v>
+      </c>
+      <c r="I10" s="10">
+        <v>40</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C11" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.108</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.188</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.246</v>
+      </c>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F13" s="3">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="J1:J4"/>
+    <mergeCell ref="J10:J13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9962,17 +10303,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -10179,17 +10520,17 @@
       <c r="I10" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -10396,17 +10737,17 @@
       <c r="I26" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" s="1">
@@ -10626,17 +10967,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -10843,17 +11184,17 @@
       <c r="I10" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -11060,17 +11401,17 @@
       <c r="I26" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" s="1">
@@ -11290,17 +11631,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -11507,17 +11848,17 @@
       <c r="I10" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -11724,17 +12065,17 @@
       <c r="I26" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" s="1">
@@ -11954,17 +12295,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -12171,17 +12512,17 @@
       <c r="I10" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -12388,17 +12729,17 @@
       <c r="I26" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" s="1">

</xml_diff>

<commit_message>
results for real classifier
too bad, need to address the data imbalance
</commit_message>
<xml_diff>
--- a/results_for_eccv/result.xlsx
+++ b/results_for_eccv/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoumengjie/Desktop/route-finder/results_for_eccv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E305C10-11E2-DA45-BE61-34326306EFD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89A4877-7FC3-B746-A0D8-0CB2B1784026}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="24700" windowHeight="14220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="24700" windowHeight="14220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSD_T_length " sheetId="1" r:id="rId1"/>
@@ -22,117 +22,7 @@
     <sheet name=" BSD_dist" sheetId="7" r:id="rId7"/>
     <sheet name="ES" sheetId="8" state="hidden" r:id="rId8"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'BSD_T_length '!$A$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'BSD_T_length '!$A$3</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'BSD_T_length '!$B$3:$I$3</definedName>
-    <definedName name="_xlchart.v1.100" hidden="1">BSD_length!$B$52:$I$52</definedName>
-    <definedName name="_xlchart.v1.101" hidden="1">BSD_length!$B$53:$I$53</definedName>
-    <definedName name="_xlchart.v1.102" hidden="1">BSD_length!$B$54:$I$54</definedName>
-    <definedName name="_xlchart.v1.103" hidden="1">BSD_length!$B$55:$I$55</definedName>
-    <definedName name="_xlchart.v1.104" hidden="1">BSD_length!$B$56:$I$56</definedName>
-    <definedName name="_xlchart.v1.105" hidden="1">BSD_length!$B$57:$I$57</definedName>
-    <definedName name="_xlchart.v1.106" hidden="1">BSD_length!$B$58:$I$58</definedName>
-    <definedName name="_xlchart.v1.107" hidden="1">BSD_length!$B$59:$I$59</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'BSD_T_length '!$B$4:$I$4</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'BSD_T_length '!$B$5:$I$5</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'BSD_T_length '!$B$6:$I$6</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'BSD_T_length '!$B$7:$I$7</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'BSD_T_length '!$B$8:$I$8</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'BSD_T_length '!$B$9:$I$9</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'BSD_T_length '!$A$10</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'BSD_T_length '!$A$3</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'BSD_T_length '!$A$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'BSD_T_length '!$A$4</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'BSD_T_length '!$A$5</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'BSD_T_length '!$A$6</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'BSD_T_length '!$A$7</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'BSD_T_length '!$A$8</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'BSD_T_length '!$A$9</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'BSD_T_length '!$B$10:$I$10</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'BSD_T_length '!$B$2:$I$2</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'BSD_T_length '!$B$3:$I$3</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'BSD_T_length '!$B$4:$I$4</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'BSD_T_length '!$B$5:$I$5</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'BSD_T_length '!$A$5</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'BSD_T_length '!$B$6:$I$6</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'BSD_T_length '!$B$7:$I$7</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'BSD_T_length '!$B$8:$I$8</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'BSD_T_length '!$B$9:$I$9</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'BSD_T_length '!$A$10</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'BSD_T_length '!$A$3</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'BSD_T_length '!$A$4</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'BSD_T_length '!$A$5</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'BSD_T_length '!$A$6</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'BSD_T_length '!$A$7</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'BSD_T_length '!$A$6</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'BSD_T_length '!$A$8</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'BSD_T_length '!$A$9</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">'BSD_T_length '!$B$10:$I$10</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'BSD_T_length '!$B$2:$I$2</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">'BSD_T_length '!$B$3:$I$3</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">'BSD_T_length '!$B$4:$I$4</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">'BSD_T_length '!$B$5:$I$5</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">'BSD_T_length '!$B$6:$I$6</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">'BSD_T_length '!$B$7:$I$7</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">'BSD_T_length '!$B$8:$I$8</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'BSD_T_length '!$A$7</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">'BSD_T_length '!$B$9:$I$9</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">BSD_length!$A$51</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">BSD_length!$A$52</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">BSD_length!$A$53</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">BSD_length!$A$54</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">BSD_length!$A$55</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">BSD_length!$A$56</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">BSD_length!$A$57</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">BSD_length!$A$58</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">BSD_length!$A$59</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'BSD_T_length '!$A$8</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">BSD_length!$B$50:$I$50</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">BSD_length!$B$51:$I$51</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">BSD_length!$B$52:$I$52</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">BSD_length!$B$53:$I$53</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">BSD_length!$B$54:$I$54</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">BSD_length!$B$55:$I$55</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">BSD_length!$B$56:$I$56</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">BSD_length!$B$57:$I$57</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">BSD_length!$B$58:$I$58</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">BSD_length!$B$59:$I$59</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'BSD_T_length '!$A$9</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">BSD_length!$A$51</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">BSD_length!$A$52</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">BSD_length!$A$53</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">BSD_length!$A$54</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">BSD_length!$A$55</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">BSD_length!$A$56</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">BSD_length!$A$57</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">BSD_length!$A$58</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">BSD_length!$A$59</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">BSD_length!$B$50:$I$50</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'BSD_T_length '!$B$10:$I$10</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">BSD_length!$B$51:$I$51</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">BSD_length!$B$52:$I$52</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">BSD_length!$B$53:$I$53</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">BSD_length!$B$54:$I$54</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">BSD_length!$B$55:$I$55</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">BSD_length!$B$56:$I$56</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">BSD_length!$B$57:$I$57</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">BSD_length!$B$58:$I$58</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">BSD_length!$B$59:$I$59</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">BSD_length!$A$51</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'BSD_T_length '!$B$2:$I$2</definedName>
-    <definedName name="_xlchart.v1.90" hidden="1">BSD_length!$A$52</definedName>
-    <definedName name="_xlchart.v1.91" hidden="1">BSD_length!$A$53</definedName>
-    <definedName name="_xlchart.v1.92" hidden="1">BSD_length!$A$54</definedName>
-    <definedName name="_xlchart.v1.93" hidden="1">BSD_length!$A$55</definedName>
-    <definedName name="_xlchart.v1.94" hidden="1">BSD_length!$A$56</definedName>
-    <definedName name="_xlchart.v1.95" hidden="1">BSD_length!$A$57</definedName>
-    <definedName name="_xlchart.v1.96" hidden="1">BSD_length!$A$58</definedName>
-    <definedName name="_xlchart.v1.97" hidden="1">BSD_length!$A$59</definedName>
-    <definedName name="_xlchart.v1.98" hidden="1">BSD_length!$B$50:$I$50</definedName>
-    <definedName name="_xlchart.v1.99" hidden="1">BSD_length!$B$51:$I$51</definedName>
-  </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -142,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="35">
   <si>
     <t>wall street with turns</t>
   </si>
@@ -245,12 +135,15 @@
   <si>
     <t>hudsonriver without turns (new test routes)</t>
   </si>
+  <si>
+    <t>BSD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -294,6 +187,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -346,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -402,14 +302,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -15101,10 +15007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15113,17 +15019,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -15384,17 +15290,17 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
@@ -15655,15 +15561,33 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="A24" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="25">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C24" s="25">
+        <v>0.122</v>
+      </c>
+      <c r="D24" s="25">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="E24" s="25">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="F24" s="25">
+        <v>0.54</v>
+      </c>
+      <c r="G24" s="25">
+        <v>0.628</v>
+      </c>
+      <c r="H24" s="25">
+        <v>0.73</v>
+      </c>
+      <c r="I24" s="25">
+        <v>0.78200000000000003</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
@@ -15688,17 +15612,17 @@
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
@@ -15958,18 +15882,47 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="C38" s="25">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="D38" s="25">
+        <v>0.192</v>
+      </c>
+      <c r="E38" s="25">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="F38" s="25">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="G38" s="25">
+        <v>0.59</v>
+      </c>
+      <c r="H38" s="25">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="I38" s="25">
+        <v>0.80600000000000005</v>
+      </c>
+    </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B43" s="1">
@@ -16229,19 +16182,48 @@
         <v>0.53200000000000003</v>
       </c>
     </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" s="25">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C52" s="25">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D52" s="25">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="E52" s="25">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="F52" s="25">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="G52" s="25">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="H52" s="25">
+        <v>0.374</v>
+      </c>
+      <c r="I52" s="25">
+        <v>0.436</v>
+      </c>
+    </row>
     <row r="54" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="21"/>
-      <c r="H55" s="21"/>
-      <c r="I55" s="21"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
     </row>
     <row r="56" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="16">
@@ -16285,16 +16267,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="21"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="22"/>
     </row>
     <row r="60" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="18"/>
@@ -16530,29 +16512,58 @@
       <c r="A68" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B68" s="23">
+      <c r="B68" s="21">
         <v>0.13</v>
       </c>
-      <c r="C68" s="23">
+      <c r="C68" s="21">
         <v>0.35599999999999998</v>
       </c>
-      <c r="D68" s="23">
+      <c r="D68" s="21">
         <v>0.55400000000000005</v>
       </c>
-      <c r="E68" s="23">
+      <c r="E68" s="21">
         <v>0.69799999999999995</v>
       </c>
-      <c r="F68" s="23">
+      <c r="F68" s="21">
         <v>0.78</v>
       </c>
-      <c r="G68" s="23">
+      <c r="G68" s="21">
         <v>0.83</v>
       </c>
-      <c r="H68" s="23">
+      <c r="H68" s="21">
         <v>0.878</v>
       </c>
-      <c r="I68" s="23">
+      <c r="I68" s="21">
         <v>0.91800000000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" s="25">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C69" s="25">
+        <v>0.08</v>
+      </c>
+      <c r="D69" s="25">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="E69" s="25">
+        <v>0.312</v>
+      </c>
+      <c r="F69" s="25">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="G69" s="25">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="H69" s="25">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="I69" s="25">
+        <v>0.628</v>
       </c>
     </row>
   </sheetData>
@@ -16584,17 +16595,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -16855,17 +16866,17 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
@@ -17155,17 +17166,17 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B33" s="1">
@@ -17455,17 +17466,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="21" t="s">
+      <c r="A49" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="21"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B50" s="1">
@@ -17757,16 +17768,16 @@
     <row r="63" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="21"/>
-      <c r="H64" s="21"/>
-      <c r="I64" s="21"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="22"/>
     </row>
     <row r="65" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="16">
@@ -17810,17 +17821,17 @@
     </row>
     <row r="67" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="70" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="21" t="s">
+      <c r="A70" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="21"/>
-      <c r="G70" s="21"/>
-      <c r="H70" s="21"/>
-      <c r="I70" s="21"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+      <c r="H70" s="22"/>
+      <c r="I70" s="22"/>
     </row>
     <row r="71" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B71" s="1">
@@ -18165,7 +18176,7 @@
       <c r="I1" s="11">
         <v>40</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="23" t="s">
         <v>13</v>
       </c>
     </row>
@@ -18197,7 +18208,7 @@
       <c r="I2" s="3">
         <v>0.30599999999999999</v>
       </c>
-      <c r="J2" s="22"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -18227,7 +18238,7 @@
       <c r="I3" s="3">
         <v>0.246</v>
       </c>
-      <c r="J3" s="22"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -18257,7 +18268,7 @@
       <c r="I4" s="3">
         <v>0.25800000000000001</v>
       </c>
-      <c r="J4" s="22"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
@@ -18311,7 +18322,7 @@
       <c r="I10" s="11">
         <v>40</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="23" t="s">
         <v>17</v>
       </c>
     </row>
@@ -18343,7 +18354,7 @@
       <c r="I11" s="8">
         <v>0.41199999999999998</v>
       </c>
-      <c r="J11" s="22"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -18373,7 +18384,7 @@
       <c r="I12" s="8">
         <v>0.246</v>
       </c>
-      <c r="J12" s="22"/>
+      <c r="J12" s="23"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -18403,7 +18414,7 @@
       <c r="I13" s="8">
         <v>0.25800000000000001</v>
       </c>
-      <c r="J13" s="22"/>
+      <c r="J13" s="23"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -18458,17 +18469,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -18675,17 +18686,17 @@
       <c r="I10" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -18892,17 +18903,17 @@
       <c r="I26" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" s="1">
@@ -19122,17 +19133,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -19339,17 +19350,17 @@
       <c r="I10" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -19556,17 +19567,17 @@
       <c r="I26" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" s="1">
@@ -19786,17 +19797,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -20003,17 +20014,17 @@
       <c r="I10" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -20220,17 +20231,17 @@
       <c r="I26" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" s="1">
@@ -20450,17 +20461,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
@@ -20667,17 +20678,17 @@
       <c r="I10" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -20884,17 +20895,17 @@
       <c r="I26" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B34" s="1">

</xml_diff>

<commit_message>
new sub results for strict criteria
</commit_message>
<xml_diff>
--- a/results_for_eccv/result.xlsx
+++ b/results_for_eccv/result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoumengjie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoumengjie/Desktop/route-finder/results_for_eccv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070D574C-E992-714E-AD54-C513E8483CD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECA7B55-FCDD-7A43-B71E-61C05BD02E88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="940" windowWidth="24700" windowHeight="14220" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="620" windowWidth="24700" windowHeight="14220" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSD_T_length " sheetId="1" r:id="rId1"/>
@@ -272,6 +272,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -281,7 +282,6 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6524,6 +6524,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.1999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.59199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68400000000000005</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6611,6 +6635,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.754</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.82399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.86199999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6698,6 +6746,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.442</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95399999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.95199999999999996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6791,6 +6863,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.34599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.79600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94599999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96399999999999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9834,8 +9930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:I42"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9847,17 +9943,17 @@
       <c r="A1" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
@@ -10139,17 +10235,17 @@
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
@@ -10268,28 +10364,28 @@
       <c r="A23" s="21">
         <v>75</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="25">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="25">
         <v>0.16800000000000001</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D23" s="25">
         <v>0.42799999999999999</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23" s="25">
         <v>0.64800000000000002</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="25">
         <v>0.81</v>
       </c>
-      <c r="G23" s="28">
+      <c r="G23" s="25">
         <v>0.92</v>
       </c>
-      <c r="H23" s="28">
+      <c r="H23" s="25">
         <v>0.96</v>
       </c>
-      <c r="I23" s="28">
+      <c r="I23" s="25">
         <v>0.97599999999999998</v>
       </c>
     </row>
@@ -10432,16 +10528,16 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
     </row>
     <row r="35" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
@@ -10728,8 +10824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A6:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:I51"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10738,17 +10834,17 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
@@ -11022,17 +11118,17 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
@@ -11341,17 +11437,17 @@
       <c r="I46"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="9"/>
@@ -11471,53 +11567,117 @@
       <c r="A52" s="2">
         <v>75</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
+      <c r="B52" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="C52" s="3">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0.68400000000000005</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>80</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
+      <c r="B53" s="3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="C53" s="3">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="G53" s="3">
+        <v>0.754</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="I53" s="3">
+        <v>0.86199999999999999</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>90</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
+      <c r="B54" s="3">
+        <v>0.122</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0.442</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="E54" s="3">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="H54" s="3">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0.95199999999999996</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>100</v>
       </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
+      <c r="B55" s="3">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0.96399999999999997</v>
+      </c>
     </row>
     <row r="56" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
@@ -11587,17 +11747,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" s="9"/>
@@ -11627,7 +11787,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="2">
@@ -11659,7 +11819,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="26"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="2">
         <v>45</v>
       </c>
@@ -11689,7 +11849,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="26"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="2">
         <v>60</v>
       </c>
@@ -11731,7 +11891,7 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2">
@@ -11763,7 +11923,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="2">
         <v>45</v>
       </c>
@@ -11793,7 +11953,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="2">
         <v>60</v>
       </c>
@@ -11835,7 +11995,7 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="2">
@@ -11867,7 +12027,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="2">
         <v>45</v>
       </c>
@@ -11897,7 +12057,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="2">
         <v>60</v>
       </c>
@@ -11939,7 +12099,7 @@
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="27" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2">
@@ -11971,7 +12131,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="26"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="2">
         <v>45</v>
       </c>
@@ -12001,7 +12161,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="26"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="2">
         <v>60</v>
       </c>

</xml_diff>